<commit_message>
fix: add multi score in audio
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -376,7 +376,7 @@
           <t>обучение</t>
         </is>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -399,6 +399,9 @@
         <is>
           <t>контент</t>
         </is>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
feat: add key words in category_aliases
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -386,12 +386,18 @@
           <t>нетворкинг</t>
         </is>
       </c>
+      <c r="I3" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t>аудитория</t>
         </is>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
fix: add link to repo in README.md
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -396,7 +396,7 @@
           <t>аудитория</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -415,6 +415,9 @@
         <is>
           <t>спорт</t>
         </is>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
feat: add telegram bot
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -416,7 +416,7 @@
           <t>спорт</t>
         </is>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -426,12 +426,18 @@
           <t>семья</t>
         </is>
       </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
           <t>проекты</t>
         </is>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>